<commit_message>
new data files after deleting a row with NAN values
</commit_message>
<xml_diff>
--- a/data/y_test.xlsx
+++ b/data/y_test.xlsx
@@ -445,7 +445,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -457,7 +457,7 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -465,7 +465,7 @@
         <v>0</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -474,15 +474,15 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -547,7 +547,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -559,7 +559,7 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -567,7 +567,7 @@
         <v>0</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -576,7 +576,7 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -584,7 +584,7 @@
         <v>0</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -593,7 +593,7 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -601,7 +601,7 @@
         <v>0</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -610,15 +610,15 @@
         <v>0</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -700,10 +700,10 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -734,7 +734,7 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -746,15 +746,15 @@
         <v>0</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -791,13 +791,13 @@
         <v>0</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24">
         <v>0</v>
       </c>
       <c r="E24">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -836,7 +836,7 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -848,7 +848,7 @@
         <v>0</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -887,7 +887,7 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -899,7 +899,7 @@
         <v>0</v>
       </c>
       <c r="E30">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -921,10 +921,10 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -938,7 +938,7 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -950,7 +950,7 @@
         <v>0</v>
       </c>
       <c r="E33">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -958,7 +958,7 @@
         <v>0</v>
       </c>
       <c r="B34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -967,7 +967,7 @@
         <v>0</v>
       </c>
       <c r="E34">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1009,7 +1009,7 @@
         <v>0</v>
       </c>
       <c r="B37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -1018,7 +1018,7 @@
         <v>0</v>
       </c>
       <c r="E37">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1060,7 +1060,7 @@
         <v>0</v>
       </c>
       <c r="B40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -1069,7 +1069,7 @@
         <v>0</v>
       </c>
       <c r="E40">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1111,7 +1111,7 @@
         <v>0</v>
       </c>
       <c r="B43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C43">
         <v>0</v>
@@ -1120,7 +1120,7 @@
         <v>0</v>
       </c>
       <c r="E43">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1142,7 +1142,7 @@
     </row>
     <row r="45" spans="1:5">
       <c r="A45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -1154,7 +1154,7 @@
         <v>0</v>
       </c>
       <c r="E45">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1162,7 +1162,7 @@
         <v>0</v>
       </c>
       <c r="B46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C46">
         <v>0</v>
@@ -1171,7 +1171,7 @@
         <v>0</v>
       </c>
       <c r="E46">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1199,13 +1199,13 @@
         <v>0</v>
       </c>
       <c r="C48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D48">
         <v>0</v>
       </c>
       <c r="E48">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1227,7 +1227,7 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -1239,15 +1239,15 @@
         <v>0</v>
       </c>
       <c r="E50">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C51">
         <v>0</v>
@@ -1264,7 +1264,7 @@
         <v>0</v>
       </c>
       <c r="B52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C52">
         <v>0</v>
@@ -1273,7 +1273,7 @@
         <v>0</v>
       </c>
       <c r="E52">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -1295,10 +1295,10 @@
     </row>
     <row r="54" spans="1:5">
       <c r="A54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C54">
         <v>0</v>
@@ -1312,10 +1312,10 @@
     </row>
     <row r="55" spans="1:5">
       <c r="A55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C55">
         <v>0</v>
@@ -1329,7 +1329,7 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B56">
         <v>0</v>
@@ -1341,7 +1341,7 @@
         <v>0</v>
       </c>
       <c r="E56">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -1349,7 +1349,7 @@
         <v>0</v>
       </c>
       <c r="B57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C57">
         <v>0</v>
@@ -1358,12 +1358,12 @@
         <v>0</v>
       </c>
       <c r="E57">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:5">
       <c r="A58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B58">
         <v>0</v>
@@ -1375,15 +1375,15 @@
         <v>0</v>
       </c>
       <c r="E58">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:5">
       <c r="A59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C59">
         <v>0</v>
@@ -1397,7 +1397,7 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B60">
         <v>0</v>
@@ -1409,15 +1409,15 @@
         <v>0</v>
       </c>
       <c r="E60">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:5">
       <c r="A61">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -1454,13 +1454,13 @@
         <v>0</v>
       </c>
       <c r="C63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D63">
         <v>0</v>
       </c>
       <c r="E63">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -1485,7 +1485,7 @@
         <v>0</v>
       </c>
       <c r="B65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C65">
         <v>0</v>
@@ -1494,12 +1494,12 @@
         <v>0</v>
       </c>
       <c r="E65">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B66">
         <v>0</v>
@@ -1511,7 +1511,7 @@
         <v>0</v>
       </c>
       <c r="E66">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -1533,7 +1533,7 @@
     </row>
     <row r="68" spans="1:5">
       <c r="A68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B68">
         <v>0</v>
@@ -1545,7 +1545,7 @@
         <v>0</v>
       </c>
       <c r="E68">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -1553,7 +1553,7 @@
         <v>0</v>
       </c>
       <c r="B69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C69">
         <v>0</v>
@@ -1562,7 +1562,7 @@
         <v>0</v>
       </c>
       <c r="E69">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -1587,7 +1587,7 @@
         <v>0</v>
       </c>
       <c r="B71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C71">
         <v>0</v>
@@ -1596,7 +1596,7 @@
         <v>0</v>
       </c>
       <c r="E71">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -1635,10 +1635,10 @@
     </row>
     <row r="74" spans="1:5">
       <c r="A74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C74">
         <v>0</v>
@@ -1669,7 +1669,7 @@
     </row>
     <row r="76" spans="1:5">
       <c r="A76">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B76">
         <v>0</v>
@@ -1681,7 +1681,7 @@
         <v>0</v>
       </c>
       <c r="E76">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -1706,7 +1706,7 @@
         <v>0</v>
       </c>
       <c r="B78">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C78">
         <v>0</v>
@@ -1715,12 +1715,12 @@
         <v>0</v>
       </c>
       <c r="E78">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:5">
       <c r="A79">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B79">
         <v>0</v>
@@ -1732,7 +1732,7 @@
         <v>0</v>
       </c>
       <c r="E79">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:5">
@@ -1757,7 +1757,7 @@
         <v>0</v>
       </c>
       <c r="B81">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C81">
         <v>0</v>
@@ -1766,7 +1766,7 @@
         <v>0</v>
       </c>
       <c r="E81">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:5">
@@ -1822,10 +1822,10 @@
     </row>
     <row r="85" spans="1:5">
       <c r="A85">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B85">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C85">
         <v>0</v>
@@ -1859,7 +1859,7 @@
         <v>0</v>
       </c>
       <c r="B87">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C87">
         <v>0</v>
@@ -1868,7 +1868,7 @@
         <v>0</v>
       </c>
       <c r="E87">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -1890,7 +1890,7 @@
     </row>
     <row r="89" spans="1:5">
       <c r="A89">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B89">
         <v>0</v>
@@ -1902,7 +1902,7 @@
         <v>0</v>
       </c>
       <c r="E89">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:5">
@@ -1924,13 +1924,13 @@
     </row>
     <row r="91" spans="1:5">
       <c r="A91">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B91">
         <v>0</v>
       </c>
       <c r="C91">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D91">
         <v>0</v>
@@ -1964,13 +1964,13 @@
         <v>0</v>
       </c>
       <c r="C93">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D93">
         <v>0</v>
       </c>
       <c r="E93">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:5">
@@ -1995,7 +1995,7 @@
         <v>0</v>
       </c>
       <c r="B95">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C95">
         <v>0</v>
@@ -2004,7 +2004,7 @@
         <v>0</v>
       </c>
       <c r="E95">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:5">
@@ -2029,10 +2029,10 @@
         <v>0</v>
       </c>
       <c r="B97">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C97">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D97">
         <v>0</v>
@@ -2043,7 +2043,7 @@
     </row>
     <row r="98" spans="1:5">
       <c r="A98">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B98">
         <v>0</v>
@@ -2055,12 +2055,12 @@
         <v>0</v>
       </c>
       <c r="E98">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:5">
       <c r="A99">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B99">
         <v>0</v>
@@ -2072,12 +2072,12 @@
         <v>0</v>
       </c>
       <c r="E99">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:5">
       <c r="A100">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B100">
         <v>0</v>
@@ -2089,7 +2089,7 @@
         <v>0</v>
       </c>
       <c r="E100">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:5">
@@ -2097,7 +2097,7 @@
         <v>0</v>
       </c>
       <c r="B101">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C101">
         <v>0</v>
@@ -2106,12 +2106,12 @@
         <v>0</v>
       </c>
       <c r="E101">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:5">
       <c r="A102">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B102">
         <v>0</v>
@@ -2123,7 +2123,7 @@
         <v>0</v>
       </c>
       <c r="E102">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:5">
@@ -2148,7 +2148,7 @@
         <v>0</v>
       </c>
       <c r="B104">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C104">
         <v>0</v>
@@ -2157,7 +2157,7 @@
         <v>0</v>
       </c>
       <c r="E104">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:5">
@@ -2199,7 +2199,7 @@
         <v>0</v>
       </c>
       <c r="B107">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C107">
         <v>0</v>
@@ -2208,12 +2208,12 @@
         <v>0</v>
       </c>
       <c r="E107">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="108" spans="1:5">
       <c r="A108">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B108">
         <v>0</v>
@@ -2225,12 +2225,12 @@
         <v>0</v>
       </c>
       <c r="E108">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109" spans="1:5">
       <c r="A109">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B109">
         <v>0</v>
@@ -2242,7 +2242,7 @@
         <v>0</v>
       </c>
       <c r="E109">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="110" spans="1:5">
@@ -2301,7 +2301,7 @@
         <v>0</v>
       </c>
       <c r="B113">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C113">
         <v>0</v>
@@ -2310,7 +2310,7 @@
         <v>0</v>
       </c>
       <c r="E113">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114" spans="1:5">
@@ -2318,7 +2318,7 @@
         <v>0</v>
       </c>
       <c r="B114">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C114">
         <v>0</v>
@@ -2327,7 +2327,7 @@
         <v>0</v>
       </c>
       <c r="E114">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115" spans="1:5">
@@ -2349,7 +2349,7 @@
     </row>
     <row r="116" spans="1:5">
       <c r="A116">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B116">
         <v>0</v>
@@ -2361,12 +2361,12 @@
         <v>0</v>
       </c>
       <c r="E116">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="117" spans="1:5">
       <c r="A117">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B117">
         <v>0</v>
@@ -2378,7 +2378,7 @@
         <v>0</v>
       </c>
       <c r="E117">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118" spans="1:5">
@@ -2417,7 +2417,7 @@
     </row>
     <row r="120" spans="1:5">
       <c r="A120">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B120">
         <v>0</v>
@@ -2429,7 +2429,7 @@
         <v>0</v>
       </c>
       <c r="E120">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="121" spans="1:5">
@@ -2437,7 +2437,7 @@
         <v>0</v>
       </c>
       <c r="B121">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C121">
         <v>0</v>
@@ -2446,7 +2446,7 @@
         <v>0</v>
       </c>
       <c r="E121">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122" spans="1:5">
@@ -2536,10 +2536,10 @@
     </row>
     <row r="127" spans="1:5">
       <c r="A127">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B127">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C127">
         <v>0</v>
@@ -2573,7 +2573,7 @@
         <v>0</v>
       </c>
       <c r="B129">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C129">
         <v>0</v>
@@ -2582,12 +2582,12 @@
         <v>0</v>
       </c>
       <c r="E129">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="130" spans="1:5">
       <c r="A130">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B130">
         <v>0</v>
@@ -2599,7 +2599,7 @@
         <v>0</v>
       </c>
       <c r="E130">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="131" spans="1:5">
@@ -2621,7 +2621,7 @@
     </row>
     <row r="132" spans="1:5">
       <c r="A132">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B132">
         <v>0</v>
@@ -2633,7 +2633,7 @@
         <v>0</v>
       </c>
       <c r="E132">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="133" spans="1:5">
@@ -2740,7 +2740,7 @@
     </row>
     <row r="139" spans="1:5">
       <c r="A139">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B139">
         <v>0</v>
@@ -2752,15 +2752,15 @@
         <v>0</v>
       </c>
       <c r="E139">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140" spans="1:5">
       <c r="A140">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B140">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C140">
         <v>0</v>
@@ -2862,7 +2862,7 @@
         <v>0</v>
       </c>
       <c r="B146">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C146">
         <v>0</v>
@@ -2871,7 +2871,7 @@
         <v>0</v>
       </c>
       <c r="E146">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="147" spans="1:5">
@@ -2879,7 +2879,7 @@
         <v>0</v>
       </c>
       <c r="B147">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C147">
         <v>0</v>
@@ -2888,7 +2888,7 @@
         <v>0</v>
       </c>
       <c r="E147">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="148" spans="1:5">
@@ -2896,7 +2896,7 @@
         <v>0</v>
       </c>
       <c r="B148">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C148">
         <v>0</v>
@@ -2905,18 +2905,18 @@
         <v>0</v>
       </c>
       <c r="E148">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="149" spans="1:5">
       <c r="A149">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B149">
         <v>0</v>
       </c>
       <c r="C149">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D149">
         <v>0</v>
@@ -2933,13 +2933,13 @@
         <v>0</v>
       </c>
       <c r="C150">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D150">
         <v>0</v>
       </c>
       <c r="E150">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="151" spans="1:5">
@@ -2947,7 +2947,7 @@
         <v>0</v>
       </c>
       <c r="B151">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C151">
         <v>0</v>
@@ -2956,12 +2956,12 @@
         <v>0</v>
       </c>
       <c r="E151">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="152" spans="1:5">
       <c r="A152">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B152">
         <v>0</v>
@@ -2973,15 +2973,15 @@
         <v>0</v>
       </c>
       <c r="E152">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="153" spans="1:5">
       <c r="A153">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B153">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C153">
         <v>0</v>
@@ -3001,13 +3001,13 @@
         <v>0</v>
       </c>
       <c r="C154">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D154">
         <v>0</v>
       </c>
       <c r="E154">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="155" spans="1:5">
@@ -3015,7 +3015,7 @@
         <v>0</v>
       </c>
       <c r="B155">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C155">
         <v>0</v>
@@ -3024,7 +3024,7 @@
         <v>0</v>
       </c>
       <c r="E155">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="156" spans="1:5">
@@ -3083,13 +3083,13 @@
         <v>0</v>
       </c>
       <c r="B159">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C159">
         <v>0</v>
       </c>
       <c r="D159">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E159">
         <v>0</v>
@@ -3120,21 +3120,21 @@
         <v>0</v>
       </c>
       <c r="C161">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D161">
         <v>0</v>
       </c>
       <c r="E161">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="162" spans="1:5">
       <c r="A162">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B162">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C162">
         <v>0</v>
@@ -3148,10 +3148,10 @@
     </row>
     <row r="163" spans="1:5">
       <c r="A163">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B163">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C163">
         <v>0</v>
@@ -3165,7 +3165,7 @@
     </row>
     <row r="164" spans="1:5">
       <c r="A164">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B164">
         <v>0</v>
@@ -3177,7 +3177,7 @@
         <v>0</v>
       </c>
       <c r="E164">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="165" spans="1:5">
@@ -3199,7 +3199,7 @@
     </row>
     <row r="166" spans="1:5">
       <c r="A166">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B166">
         <v>0</v>
@@ -3211,7 +3211,7 @@
         <v>0</v>
       </c>
       <c r="E166">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="167" spans="1:5">
@@ -3250,7 +3250,7 @@
     </row>
     <row r="169" spans="1:5">
       <c r="A169">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B169">
         <v>0</v>
@@ -3262,15 +3262,15 @@
         <v>0</v>
       </c>
       <c r="E169">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="170" spans="1:5">
       <c r="A170">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B170">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C170">
         <v>0</v>
@@ -3301,7 +3301,7 @@
     </row>
     <row r="172" spans="1:5">
       <c r="A172">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B172">
         <v>0</v>
@@ -3313,7 +3313,7 @@
         <v>0</v>
       </c>
       <c r="E172">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="173" spans="1:5">
@@ -3352,10 +3352,10 @@
     </row>
     <row r="175" spans="1:5">
       <c r="A175">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B175">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C175">
         <v>0</v>
@@ -3369,10 +3369,10 @@
     </row>
     <row r="176" spans="1:5">
       <c r="A176">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B176">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C176">
         <v>0</v>
@@ -3389,7 +3389,7 @@
         <v>0</v>
       </c>
       <c r="B177">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C177">
         <v>0</v>
@@ -3398,7 +3398,7 @@
         <v>0</v>
       </c>
       <c r="E177">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="178" spans="1:5">
@@ -3457,7 +3457,7 @@
         <v>0</v>
       </c>
       <c r="B181">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C181">
         <v>0</v>
@@ -3466,12 +3466,12 @@
         <v>0</v>
       </c>
       <c r="E181">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="182" spans="1:5">
       <c r="A182">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B182">
         <v>0</v>
@@ -3483,15 +3483,15 @@
         <v>0</v>
       </c>
       <c r="E182">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="183" spans="1:5">
       <c r="A183">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B183">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C183">
         <v>0</v>
@@ -3508,7 +3508,7 @@
         <v>0</v>
       </c>
       <c r="B184">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C184">
         <v>0</v>
@@ -3517,12 +3517,12 @@
         <v>0</v>
       </c>
       <c r="E184">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="185" spans="1:5">
       <c r="A185">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B185">
         <v>0</v>
@@ -3534,18 +3534,18 @@
         <v>0</v>
       </c>
       <c r="E185">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="186" spans="1:5">
       <c r="A186">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B186">
         <v>0</v>
       </c>
       <c r="C186">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D186">
         <v>0</v>
@@ -3559,7 +3559,7 @@
         <v>0</v>
       </c>
       <c r="B187">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C187">
         <v>0</v>
@@ -3568,12 +3568,12 @@
         <v>0</v>
       </c>
       <c r="E187">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="188" spans="1:5">
       <c r="A188">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B188">
         <v>0</v>
@@ -3585,7 +3585,7 @@
         <v>0</v>
       </c>
       <c r="E188">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="189" spans="1:5">
@@ -3593,7 +3593,7 @@
         <v>0</v>
       </c>
       <c r="B189">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C189">
         <v>0</v>
@@ -3602,7 +3602,7 @@
         <v>0</v>
       </c>
       <c r="E189">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="190" spans="1:5">
@@ -3610,10 +3610,10 @@
         <v>0</v>
       </c>
       <c r="B190">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C190">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D190">
         <v>0</v>
@@ -3627,7 +3627,7 @@
         <v>0</v>
       </c>
       <c r="B191">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C191">
         <v>0</v>
@@ -3636,7 +3636,7 @@
         <v>0</v>
       </c>
       <c r="E191">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="192" spans="1:5">
@@ -3729,10 +3729,10 @@
         <v>0</v>
       </c>
       <c r="B197">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C197">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D197">
         <v>0</v>
@@ -3760,7 +3760,7 @@
     </row>
     <row r="199" spans="1:5">
       <c r="A199">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B199">
         <v>0</v>
@@ -3772,7 +3772,7 @@
         <v>0</v>
       </c>
       <c r="E199">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="200" spans="1:5">
@@ -3797,7 +3797,7 @@
         <v>0</v>
       </c>
       <c r="B201">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C201">
         <v>0</v>
@@ -3806,7 +3806,7 @@
         <v>0</v>
       </c>
       <c r="E201">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="202" spans="1:5">
@@ -3814,7 +3814,7 @@
         <v>0</v>
       </c>
       <c r="B202">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C202">
         <v>0</v>
@@ -3823,12 +3823,12 @@
         <v>0</v>
       </c>
       <c r="E202">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="203" spans="1:5">
       <c r="A203">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B203">
         <v>0</v>
@@ -3840,7 +3840,7 @@
         <v>0</v>
       </c>
       <c r="E203">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="204" spans="1:5">
@@ -3848,7 +3848,7 @@
         <v>0</v>
       </c>
       <c r="B204">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C204">
         <v>0</v>
@@ -3857,7 +3857,7 @@
         <v>0</v>
       </c>
       <c r="E204">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="205" spans="1:5">
@@ -3865,7 +3865,7 @@
         <v>0</v>
       </c>
       <c r="B205">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C205">
         <v>0</v>
@@ -3874,7 +3874,7 @@
         <v>0</v>
       </c>
       <c r="E205">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="206" spans="1:5">
@@ -3896,10 +3896,10 @@
     </row>
     <row r="207" spans="1:5">
       <c r="A207">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B207">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C207">
         <v>0</v>
@@ -3913,7 +3913,7 @@
     </row>
     <row r="208" spans="1:5">
       <c r="A208">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B208">
         <v>0</v>
@@ -3925,12 +3925,12 @@
         <v>0</v>
       </c>
       <c r="E208">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="209" spans="1:5">
       <c r="A209">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B209">
         <v>0</v>
@@ -3942,15 +3942,15 @@
         <v>0</v>
       </c>
       <c r="E209">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="210" spans="1:5">
       <c r="A210">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B210">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C210">
         <v>0</v>
@@ -3967,7 +3967,7 @@
         <v>0</v>
       </c>
       <c r="B211">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C211">
         <v>0</v>
@@ -3976,12 +3976,12 @@
         <v>0</v>
       </c>
       <c r="E211">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="212" spans="1:5">
       <c r="A212">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B212">
         <v>0</v>
@@ -3993,12 +3993,12 @@
         <v>0</v>
       </c>
       <c r="E212">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="213" spans="1:5">
       <c r="A213">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B213">
         <v>0</v>
@@ -4010,7 +4010,7 @@
         <v>0</v>
       </c>
       <c r="E213">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="214" spans="1:5">
@@ -4018,7 +4018,7 @@
         <v>0</v>
       </c>
       <c r="B214">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C214">
         <v>0</v>
@@ -4027,7 +4027,7 @@
         <v>0</v>
       </c>
       <c r="E214">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="215" spans="1:5">
@@ -4069,7 +4069,7 @@
         <v>0</v>
       </c>
       <c r="B217">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C217">
         <v>0</v>
@@ -4078,15 +4078,15 @@
         <v>0</v>
       </c>
       <c r="E217">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="218" spans="1:5">
       <c r="A218">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B218">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C218">
         <v>0</v>
@@ -4106,18 +4106,18 @@
         <v>0</v>
       </c>
       <c r="C219">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D219">
         <v>0</v>
       </c>
       <c r="E219">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="220" spans="1:5">
       <c r="A220">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B220">
         <v>0</v>
@@ -4129,12 +4129,12 @@
         <v>0</v>
       </c>
       <c r="E220">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="221" spans="1:5">
       <c r="A221">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B221">
         <v>0</v>
@@ -4146,7 +4146,7 @@
         <v>0</v>
       </c>
       <c r="E221">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="222" spans="1:5">
@@ -4154,7 +4154,7 @@
         <v>0</v>
       </c>
       <c r="B222">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C222">
         <v>0</v>
@@ -4163,7 +4163,7 @@
         <v>0</v>
       </c>
       <c r="E222">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>